<commit_message>
Fixed camera DSL issues
</commit_message>
<xml_diff>
--- a/auto/other/UIAutomation/Hybrid_TestNG_Framework/src/com/xls/EBManual_Camera_Front_JS.xlsx
+++ b/auto/other/UIAutomation/Hybrid_TestNG_Framework/src/com/xls/EBManual_Camera_Front_JS.xlsx
@@ -154,20 +154,6 @@
 validate1;
 link_Click(camera_front_link);
 validate2;
-SelectTestToRun(VT285_0034a_string);
-ClickRunTest(runtest_top_xpath);
-wait(2);
-validate3;
-ClickRunTest(runtest_bottom_xpath);
-wait(4);
-sendKeyEvents(SOFTBACK);
-validate4;</t>
-  </si>
-  <si>
-    <t>wait(5);
-validate1;
-link_Click(camera_front_link);
-validate2;
 SelectTestToRun(VT285_0035a_string);
 ClickRunTest(runtest_top_xpath);
 wait(2);
@@ -721,6 +707,20 @@
 {
 validate_AppMinimized=com.symbol.enterprisebrowser
 };</t>
+  </si>
+  <si>
+    <t>wait(5);
+validate1;
+link_Click(camera_front_link);
+validate2;
+SelectTestToRun(VT285_0034a_string);
+ClickRunTest(runtest_top_xpath);
+wait(2);
+validate3;
+ClickRunTest(runtest_bottom_xpath);
+wait(4);
+press_Key(Back);
+validate4;</t>
   </si>
 </sst>
 </file>
@@ -1232,8 +1232,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1330,7 +1330,7 @@
         <v>33</v>
       </c>
       <c r="H3" s="13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I3" s="14"/>
       <c r="J3" s="14"/>
@@ -1354,10 +1354,10 @@
         <v>1</v>
       </c>
       <c r="G4" s="13" t="s">
-        <v>34</v>
+        <v>65</v>
       </c>
       <c r="H4" s="13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I4" s="10"/>
       <c r="J4" s="10"/>
@@ -1381,10 +1381,10 @@
         <v>1</v>
       </c>
       <c r="G5" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H5" s="13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I5" s="10"/>
       <c r="J5" s="10"/>
@@ -1407,10 +1407,10 @@
         <v>1</v>
       </c>
       <c r="G6" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H6" s="13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I6" s="10"/>
       <c r="J6" s="10"/>
@@ -1434,10 +1434,10 @@
         <v>1</v>
       </c>
       <c r="G7" s="13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H7" s="13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I7" s="10"/>
       <c r="J7" s="10"/>
@@ -1461,10 +1461,10 @@
         <v>1</v>
       </c>
       <c r="G8" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H8" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I8" s="10"/>
       <c r="J8" s="10"/>
@@ -1491,7 +1491,7 @@
         <v>32</v>
       </c>
       <c r="H9" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I9" s="10"/>
       <c r="J9" s="10"/>
@@ -1515,10 +1515,10 @@
         <v>1</v>
       </c>
       <c r="G10" s="13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H10" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I10" s="10"/>
       <c r="J10" s="10"/>
@@ -1542,10 +1542,10 @@
         <v>1</v>
       </c>
       <c r="G11" s="13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H11" s="13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I11" s="14"/>
       <c r="J11" s="14"/>
@@ -1569,10 +1569,10 @@
         <v>1</v>
       </c>
       <c r="G12" s="13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H12" s="13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I12" s="11"/>
       <c r="J12" s="11"/>
@@ -1595,10 +1595,10 @@
         <v>1</v>
       </c>
       <c r="G13" s="13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H13" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I13" s="11"/>
       <c r="J13" s="11"/>
@@ -1621,10 +1621,10 @@
         <v>1</v>
       </c>
       <c r="G14" s="13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H14" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I14" s="11"/>
       <c r="J14" s="11"/>
@@ -1647,10 +1647,10 @@
         <v>1</v>
       </c>
       <c r="G15" s="13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H15" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I15" s="14"/>
       <c r="J15" s="14"/>
@@ -1674,10 +1674,10 @@
         <v>1</v>
       </c>
       <c r="G16" s="13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H16" s="13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I16" s="10"/>
       <c r="J16" s="10"/>
@@ -1700,10 +1700,10 @@
         <v>1</v>
       </c>
       <c r="G17" s="13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H17" s="13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I17" s="14"/>
       <c r="J17" s="14"/>
@@ -1727,10 +1727,10 @@
         <v>1</v>
       </c>
       <c r="G18" s="13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H18" s="13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I18" s="14"/>
       <c r="J18" s="14"/>
@@ -1754,10 +1754,10 @@
         <v>1</v>
       </c>
       <c r="G19" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="H19" s="13" t="s">
         <v>64</v>
-      </c>
-      <c r="H19" s="13" t="s">
-        <v>65</v>
       </c>
       <c r="I19" s="14"/>
       <c r="J19" s="14"/>

</xml_diff>